<commit_message>
Look changes 4 and logic rearrangement 4
</commit_message>
<xml_diff>
--- a/outputs/all_logs.xlsx
+++ b/outputs/all_logs.xlsx
@@ -16,7 +16,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All_Logs'!$A$1:$D$315</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Unique_EventCodes'!$A$1:$D$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Log_Details_From_SWIFT'!$A$1:$C$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Merged_Summary'!$A$1:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Merged_Summary'!$A$1:$H$7</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -7430,7 +7430,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="24" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
     <col width="8" customWidth="1" min="3" max="3"/>
     <col width="50" customWidth="1" min="4" max="4"/>
@@ -7461,7 +7461,7 @@
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
         <is>
-          <t>No_AMH_Log_Code</t>
+          <t>AMH-REP-00000</t>
         </is>
       </c>
       <c r="B2" s="7" t="inlineStr">
@@ -7476,14 +7476,14 @@
       </c>
       <c r="D2" s="7" t="inlineStr">
         <is>
-          <t>- service-2025-10-28T00:00:00.000Z MB0749 Housekeeping task [cleanup-completed-workflow] started.</t>
+          <t>Report with definition 'Non-Final-Transactions' is executed by user: Everflow</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="inlineStr">
         <is>
-          <t>[AMH-REP-00000]</t>
+          <t>AMH-SVC-000160</t>
         </is>
       </c>
       <c r="B3" s="7" t="inlineStr">
@@ -7493,19 +7493,19 @@
       </c>
       <c r="C3" s="7" t="inlineStr">
         <is>
-          <t>INFO</t>
+          <t>WARN</t>
         </is>
       </c>
       <c r="D3" s="7" t="inlineStr">
         <is>
-          <t>Report with definition 'Non-Final-Transactions' is executed by user: Everflow</t>
+          <t>Alerted service for SnF Queue rbosgb21_finplussrp1ll!pip:0923045, using Output Channel Dnbsop21 [p:0923045].</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="7" t="inlineStr">
         <is>
-          <t>[AMH-SVC-000160]</t>
+          <t>AMH-SWF-00501</t>
         </is>
       </c>
       <c r="B4" s="7" t="inlineStr">
@@ -7515,19 +7515,19 @@
       </c>
       <c r="C4" s="7" t="inlineStr">
         <is>
-          <t>WARN</t>
+          <t>ERROR</t>
         </is>
       </c>
       <c r="D4" s="7" t="inlineStr">
         <is>
-          <t>Alerted service for SnF Queue rbosgb21_finplussrp1ll!pip:0923045, using Output Channel Dnbsop21 [p:0923045].</t>
+          <t>SnF session lost for SnF Queue rbosgb21_finplussrp1ll!pip:0923047, SAG Connection:SA_SAG3_LNI</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="inlineStr">
         <is>
-          <t>[AMH-SWF-00501]</t>
+          <t>AMH-SWF-00520</t>
         </is>
       </c>
       <c r="B5" s="7" t="inlineStr">
@@ -7542,14 +7542,14 @@
       </c>
       <c r="D5" s="7" t="inlineStr">
         <is>
-          <t>SnF session lost for SnF Queue rbosgb21_finplussrp1ll!pip:0923047, SAG Connection:SA_SAG3_LNI</t>
+          <t>SnF session lost for SnF Queue rbosgb21_finpllussrp1ll!pip:0923045, using Output Channel Dnbsop21 [p:0923045], reason:SnF Session was closed. Severity: Logic. Parameters [Parameters: [Parameter: [statusAttributes[0] code=Sw.Snf.InvalidSessionId, text=The session identifier is not valid or does not match the current session identifier on the queue, the session has been closed. severity=logic, parameters=[Parameters [Parameter: [Parameter: rbosgb21_finplussrpl1ll!pip:0923251], action=Check that the session identifier is correct or reacquire the queue. ] SAG Connection:SA_SAG1_LNI</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="inlineStr">
         <is>
-          <t>[AMH-SWF-00520]</t>
+          <t>AMH-USERACTION-00027</t>
         </is>
       </c>
       <c r="B6" s="7" t="inlineStr">
@@ -7559,19 +7559,19 @@
       </c>
       <c r="C6" s="7" t="inlineStr">
         <is>
-          <t>ERROR</t>
+          <t>INFO</t>
         </is>
       </c>
       <c r="D6" s="7" t="inlineStr">
         <is>
-          <t>SnF session lost for SnF Queue rbosgb21_finpllussrp1ll!pip:0923045, using Output Channel Dnbsop21 [p:0923045], reason:SnF Session was closed. Severity: Logic. Parameters [Parameters: [Parameter: [statusAttributes[0] code=Sw.Snf.InvalidSessionId, text=The session identifier is not valid or does not match the current session identifier on the queue, the session has been closed. severity=logic, parameters=[Parameters [Parameter: [Parameter: rbosgb21_finplussrpl1ll!pip:0923251], action=Check that the session identifier is correct or reacquire the queue. ] SAG Connection:SA_SAG1_LNI</t>
+          <t>- service-2025-10-28T00:00:00.000Z  The System Job 'Zenabup-completed-workflow' was executed by user service</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="inlineStr">
         <is>
-          <t>[AMH-USERACTION-00027]</t>
+          <t>No_AMH_Log_Code</t>
         </is>
       </c>
       <c r="B7" s="7" t="inlineStr">
@@ -7586,7 +7586,7 @@
       </c>
       <c r="D7" s="7" t="inlineStr">
         <is>
-          <t>- service-2025-10-28T00:00:00.000Z  The System Job 'Zenabup-completed-workflow' was executed by user service</t>
+          <t>- service-2025-10-28T00:00:00.000Z MB0749 Housekeeping task [cleanup-completed-workflow] started.</t>
         </is>
       </c>
     </row>
@@ -7636,7 +7636,7 @@
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
         <is>
-          <t>No_AMH_Log_Code</t>
+          <t>AMH-REP-00000</t>
         </is>
       </c>
       <c r="B2" s="7" t="inlineStr">
@@ -7653,85 +7653,85 @@
     <row r="3">
       <c r="A3" s="7" t="inlineStr">
         <is>
-          <t>AMH-REP-00000</t>
+          <t>AMH-SVC-000160</t>
         </is>
       </c>
       <c r="B3" s="7" t="inlineStr">
         <is>
-          <t>Data not available in Official SWIFT Log Guide</t>
+          <t>Alerted service {serviceCode} on LN {logicalNode} and PN {physicalNode}: {message}</t>
         </is>
       </c>
       <c r="C3" s="7" t="inlineStr">
         <is>
-          <t>Data not available in Official SWIFT Log Guide</t>
+          <t>service in alerted state.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="7" t="inlineStr">
         <is>
-          <t>AMH-SVC-000160</t>
+          <t>AMH-SWF-00501</t>
         </is>
       </c>
       <c r="B4" s="7" t="inlineStr">
         <is>
-          <t>Alerted service {serviceCode} on LN {logicalNode} and PN {physicalNode}: {message}</t>
+          <t>Data not available in Official SWIFT Log Guide</t>
         </is>
       </c>
       <c r="C4" s="7" t="inlineStr">
         <is>
-          <t>service in alerted state.</t>
+          <t>Data not available in Official SWIFT Log Guide</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="inlineStr">
         <is>
-          <t>AMH-SWF-00501</t>
+          <t>AMH-SWF-00520</t>
         </is>
       </c>
       <c r="B5" s="7" t="inlineStr">
         <is>
-          <t>Data not available in Official SWIFT Log Guide</t>
+          <t>SnF session lost for {object}: {sessionId}, reason:{reason}, SAG Connection:{sagConnection}</t>
         </is>
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
-          <t>Data not available in Official SWIFT Log Guide</t>
+          <t>SnF session stopped</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="inlineStr">
         <is>
-          <t>AMH-SWF-00520</t>
+          <t>AMH-USERACTION-00027</t>
         </is>
       </c>
       <c r="B6" s="7" t="inlineStr">
         <is>
-          <t>SnF session lost for {object}: {sessionId}, reason:{reason}, SAG Connection:{sagConnection}</t>
+          <t>The {EntityName} {Code} was executed by user {User}</t>
         </is>
       </c>
       <c r="C6" s="7" t="inlineStr">
         <is>
-          <t>SnF session stopped</t>
+          <t>A user executed entity code</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="inlineStr">
         <is>
-          <t>AMH-USERACTION-00027</t>
+          <t>No_AMH_Log_Code</t>
         </is>
       </c>
       <c r="B7" s="7" t="inlineStr">
         <is>
-          <t>The {EntityName} {Code} was executed by user {User}</t>
+          <t>Data not available in Official SWIFT Log Guide</t>
         </is>
       </c>
       <c r="C7" s="7" t="inlineStr">
         <is>
-          <t>A user executed entity code</t>
+          <t>Data not available in Official SWIFT Log Guide</t>
         </is>
       </c>
     </row>
@@ -7747,7 +7747,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -7756,13 +7756,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="1" max="1"/>
     <col width="8" customWidth="1" min="2" max="2"/>
     <col width="30" customWidth="1" min="3" max="3"/>
     <col width="28" customWidth="1" min="4" max="4"/>
     <col width="29" customWidth="1" min="5" max="5"/>
     <col width="22" customWidth="1" min="6" max="6"/>
-    <col width="48" customWidth="1" min="7" max="7"/>
+    <col width="93" customWidth="1" min="7" max="7"/>
     <col width="48" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
@@ -7815,7 +7815,7 @@
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
         <is>
-          <t>No_AMH_Log_Code</t>
+          <t>AMH-REP-00000</t>
         </is>
       </c>
       <c r="B2" s="7" t="inlineStr">
@@ -7838,8 +7838,138 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>AMH-SVC-000160</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="inlineStr">
+        <is>
+          <t>WARN</t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="n"/>
+      <c r="D3" s="7" t="n"/>
+      <c r="E3" s="7" t="n"/>
+      <c r="F3" s="7" t="n"/>
+      <c r="G3" s="7" t="inlineStr">
+        <is>
+          <t>Alerted service {serviceCode} on LN {logicalNode} and PN {physicalNode}: {message}</t>
+        </is>
+      </c>
+      <c r="H3" s="7" t="inlineStr">
+        <is>
+          <t>service in alerted state.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>AMH-SWF-00501</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="inlineStr">
+        <is>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="C4" s="7" t="n"/>
+      <c r="D4" s="7" t="n"/>
+      <c r="E4" s="7" t="n"/>
+      <c r="F4" s="7" t="n"/>
+      <c r="G4" s="7" t="inlineStr">
+        <is>
+          <t>Data not available in Official SWIFT Log Guide</t>
+        </is>
+      </c>
+      <c r="H4" s="7" t="inlineStr">
+        <is>
+          <t>Data not available in Official SWIFT Log Guide</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>AMH-SWF-00520</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>ERROR</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="n"/>
+      <c r="D5" s="7" t="n"/>
+      <c r="E5" s="7" t="n"/>
+      <c r="F5" s="7" t="n"/>
+      <c r="G5" s="7" t="inlineStr">
+        <is>
+          <t>SnF session lost for {object}: {sessionId}, reason:{reason}, SAG Connection:{sagConnection}</t>
+        </is>
+      </c>
+      <c r="H5" s="7" t="inlineStr">
+        <is>
+          <t>SnF session stopped</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>AMH-USERACTION-00027</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="C6" s="7" t="n"/>
+      <c r="D6" s="7" t="n"/>
+      <c r="E6" s="7" t="n"/>
+      <c r="F6" s="7" t="n"/>
+      <c r="G6" s="7" t="inlineStr">
+        <is>
+          <t>The {EntityName} {Code} was executed by user {User}</t>
+        </is>
+      </c>
+      <c r="H6" s="7" t="inlineStr">
+        <is>
+          <t>A user executed entity code</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>No_AMH_Log_Code</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="C7" s="7" t="n"/>
+      <c r="D7" s="7" t="n"/>
+      <c r="E7" s="7" t="n"/>
+      <c r="F7" s="7" t="n"/>
+      <c r="G7" s="7" t="inlineStr">
+        <is>
+          <t>Data not available in Official SWIFT Log Guide</t>
+        </is>
+      </c>
+      <c r="H7" s="7" t="inlineStr">
+        <is>
+          <t>Data not available in Official SWIFT Log Guide</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H2"/>
+  <autoFilter ref="A1:H7"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>